<commit_message>
Armatiek: Metamodel voor OpenAPI toegevoegd.
Dit metamodel kan worden geincludeerd in metamodellen van orhbganisaties
tbv. OpenAPI generatie.

Improvement.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Armatiek/props/Armatiek.xlsx
+++ b/src/main/resources/input/Armatiek/props/Armatiek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Armatiek\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7D751D-516F-4AA7-BD00-59ACFF486C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5944F6FC-89E0-43DD-891E-E82D741114D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="373">
   <si>
     <t>Name</t>
   </si>
@@ -1130,6 +1130,21 @@
   </si>
   <si>
     <t>includedoclist</t>
+  </si>
+  <si>
+    <t>OPENAPI: uitgebreid</t>
+  </si>
+  <si>
+    <t>OpenAPI</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>API</t>
   </si>
 </sst>
 </file>
@@ -1604,11 +1619,11 @@
   </sheetPr>
   <dimension ref="A1:T133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="F65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1632,9 +1647,10 @@
     <col min="17" max="17" width="15.765625" customWidth="1"/>
     <col min="18" max="18" width="16.07421875" customWidth="1"/>
     <col min="19" max="19" width="4.4609375" style="17" customWidth="1"/>
+    <col min="20" max="20" width="16.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1686,8 +1702,11 @@
         <v>253</v>
       </c>
       <c r="S1" s="12"/>
-    </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="T1" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="2"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2" t="s">
@@ -1722,8 +1741,11 @@
         <v>318</v>
       </c>
       <c r="S2" s="13"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="T2" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>156</v>
       </c>
@@ -1743,7 +1765,7 @@
       <c r="M3" s="14"/>
       <c r="S3" s="14"/>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1788,7 @@
       <c r="M4" s="14"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1789,7 +1811,7 @@
       <c r="M5" s="14"/>
       <c r="S5" s="14"/>
     </row>
-    <row r="6" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>159</v>
       </c>
@@ -1809,7 +1831,7 @@
       <c r="M6" s="14"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
@@ -1829,7 +1851,7 @@
       <c r="M7" s="14"/>
       <c r="S7" s="14"/>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1838,7 +1860,7 @@
       <c r="M8" s="14"/>
       <c r="S8" s="14"/>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>336</v>
       </c>
@@ -1861,7 +1883,7 @@
       <c r="M9" s="14"/>
       <c r="S9" s="14"/>
     </row>
-    <row r="10" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>162</v>
       </c>
@@ -1884,7 +1906,7 @@
       <c r="M10" s="14"/>
       <c r="S10" s="14"/>
     </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1907,7 +1929,7 @@
       <c r="M11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>164</v>
       </c>
@@ -1927,7 +1949,7 @@
       <c r="M12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>136</v>
       </c>
@@ -1950,7 +1972,7 @@
       <c r="M13" s="14"/>
       <c r="S13" s="14"/>
     </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>244</v>
       </c>
@@ -1973,7 +1995,7 @@
       <c r="M14" s="14"/>
       <c r="S14" s="14"/>
     </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1996,7 +2018,7 @@
       <c r="M15" s="14"/>
       <c r="S15" s="14"/>
     </row>
-    <row r="16" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -2808,7 +2830,7 @@
       <c r="M48" s="14"/>
       <c r="S48" s="14"/>
     </row>
-    <row r="49" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="21" t="s">
         <v>51</v>
       </c>
@@ -2831,7 +2853,7 @@
       <c r="M49" s="14"/>
       <c r="S49" s="14"/>
     </row>
-    <row r="50" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -2840,7 +2862,7 @@
       <c r="M50" s="14"/>
       <c r="S50" s="14"/>
     </row>
-    <row r="51" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>178</v>
       </c>
@@ -2860,7 +2882,7 @@
       <c r="M51" s="14"/>
       <c r="S51" s="14"/>
     </row>
-    <row r="52" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2883,7 +2905,7 @@
       <c r="M52" s="14"/>
       <c r="S52" s="14"/>
     </row>
-    <row r="53" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -2906,7 +2928,7 @@
       <c r="M53" s="14"/>
       <c r="S53" s="14"/>
     </row>
-    <row r="54" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>221</v>
       </c>
@@ -2922,7 +2944,7 @@
       <c r="M54" s="15"/>
       <c r="S54" s="15"/>
     </row>
-    <row r="55" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>181</v>
       </c>
@@ -2945,7 +2967,7 @@
       <c r="M55" s="14"/>
       <c r="S55" s="14"/>
     </row>
-    <row r="56" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>183</v>
       </c>
@@ -2968,7 +2990,7 @@
       <c r="M56" s="14"/>
       <c r="S56" s="14"/>
     </row>
-    <row r="57" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -2991,7 +3013,7 @@
       <c r="M57" s="14"/>
       <c r="S57" s="14"/>
     </row>
-    <row r="58" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -3014,7 +3036,7 @@
       <c r="M58" s="14"/>
       <c r="S58" s="14"/>
     </row>
-    <row r="59" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>62</v>
       </c>
@@ -3037,7 +3059,7 @@
       <c r="M59" s="14"/>
       <c r="S59" s="14"/>
     </row>
-    <row r="60" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>186</v>
       </c>
@@ -3060,7 +3082,7 @@
       <c r="M60" s="14"/>
       <c r="S60" s="14"/>
     </row>
-    <row r="61" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>315</v>
       </c>
@@ -3086,7 +3108,7 @@
       <c r="M61" s="14"/>
       <c r="S61" s="14"/>
     </row>
-    <row r="62" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A62" s="11" t="s">
         <v>279</v>
       </c>
@@ -3116,8 +3138,9 @@
       <c r="Q62" s="11"/>
       <c r="R62" s="11"/>
       <c r="S62" s="16"/>
-    </row>
-    <row r="63" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T62" s="11"/>
+    </row>
+    <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>281</v>
       </c>
@@ -3140,7 +3163,7 @@
       <c r="M63" s="14"/>
       <c r="S63" s="14"/>
     </row>
-    <row r="64" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>285</v>
       </c>
@@ -3170,8 +3193,9 @@
       <c r="Q64" s="20"/>
       <c r="R64" s="20"/>
       <c r="S64" s="14"/>
-    </row>
-    <row r="65" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T64" s="20"/>
+    </row>
+    <row r="65" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>188</v>
       </c>
@@ -3191,7 +3215,7 @@
       <c r="M65" s="14"/>
       <c r="S65" s="14"/>
     </row>
-    <row r="66" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>293</v>
       </c>
@@ -3214,7 +3238,7 @@
       <c r="M66" s="14"/>
       <c r="S66" s="14"/>
     </row>
-    <row r="67" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>294</v>
       </c>
@@ -3237,7 +3261,7 @@
       <c r="M67" s="14"/>
       <c r="S67" s="14"/>
     </row>
-    <row r="68" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="11" t="s">
         <v>241</v>
       </c>
@@ -3269,8 +3293,9 @@
       <c r="Q68" s="11"/>
       <c r="R68" s="11"/>
       <c r="S68" s="16"/>
-    </row>
-    <row r="69" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T68" s="11"/>
+    </row>
+    <row r="69" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>190</v>
       </c>
@@ -3293,7 +3318,7 @@
       <c r="M69" s="14"/>
       <c r="S69" s="14"/>
     </row>
-    <row r="70" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
@@ -3316,7 +3341,7 @@
       <c r="M70" s="14"/>
       <c r="S70" s="14"/>
     </row>
-    <row r="71" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>367</v>
       </c>
@@ -3336,7 +3361,7 @@
       <c r="M71" s="14"/>
       <c r="S71" s="14"/>
     </row>
-    <row r="72" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>288</v>
       </c>
@@ -3359,7 +3384,7 @@
       <c r="M72" s="14"/>
       <c r="S72" s="14"/>
     </row>
-    <row r="73" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>66</v>
       </c>
@@ -3382,7 +3407,7 @@
       <c r="M73" s="14"/>
       <c r="S73" s="14"/>
     </row>
-    <row r="74" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>262</v>
       </c>
@@ -3405,7 +3430,7 @@
       <c r="M74" s="14"/>
       <c r="S74" s="14"/>
     </row>
-    <row r="75" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>339</v>
       </c>
@@ -3428,7 +3453,7 @@
       <c r="M75" s="14"/>
       <c r="S75" s="14"/>
     </row>
-    <row r="76" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>69</v>
       </c>
@@ -3451,7 +3476,7 @@
       <c r="M76" s="14"/>
       <c r="S76" s="14"/>
     </row>
-    <row r="77" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
@@ -3474,7 +3499,7 @@
       <c r="M77" s="14"/>
       <c r="S77" s="14"/>
     </row>
-    <row r="78" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>193</v>
       </c>
@@ -3497,7 +3522,7 @@
       <c r="M78" s="14"/>
       <c r="S78" s="14"/>
     </row>
-    <row r="79" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>254</v>
       </c>
@@ -3520,7 +3545,7 @@
       <c r="M79" s="14"/>
       <c r="S79" s="14"/>
     </row>
-    <row r="80" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>73</v>
       </c>
@@ -3540,7 +3565,7 @@
       <c r="M80" s="14"/>
       <c r="S80" s="14"/>
     </row>
-    <row r="81" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>355</v>
       </c>
@@ -3562,8 +3587,11 @@
       <c r="G81" s="14"/>
       <c r="M81" s="14"/>
       <c r="S81" s="14"/>
-    </row>
-    <row r="82" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T81" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>352</v>
       </c>
@@ -3585,8 +3613,11 @@
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
       <c r="S82" s="14"/>
-    </row>
-    <row r="83" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T82" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>353</v>
       </c>
@@ -3635,8 +3666,11 @@
         <v>351</v>
       </c>
       <c r="S83" s="14"/>
-    </row>
-    <row r="84" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T83" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>354</v>
       </c>
@@ -3655,8 +3689,11 @@
       <c r="G84" s="14"/>
       <c r="M84" s="14"/>
       <c r="S84" s="14"/>
-    </row>
-    <row r="85" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T84" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>196</v>
       </c>
@@ -3676,7 +3713,7 @@
       <c r="M85" s="14"/>
       <c r="S85" s="14"/>
     </row>
-    <row r="86" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>329</v>
       </c>
@@ -3699,7 +3736,7 @@
       <c r="M86" s="14"/>
       <c r="S86" s="14"/>
     </row>
-    <row r="87" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>331</v>
       </c>
@@ -3722,7 +3759,7 @@
       <c r="M87" s="14"/>
       <c r="S87" s="14"/>
     </row>
-    <row r="88" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>332</v>
       </c>
@@ -3745,7 +3782,7 @@
       <c r="M88" s="14"/>
       <c r="S88" s="14"/>
     </row>
-    <row r="89" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="5" t="s">
         <v>75</v>
       </c>
@@ -3768,7 +3805,7 @@
       <c r="M89" s="14"/>
       <c r="S89" s="14"/>
     </row>
-    <row r="90" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>298</v>
       </c>
@@ -3800,8 +3837,9 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
       <c r="S90" s="14"/>
-    </row>
-    <row r="91" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T90" s="1"/>
+    </row>
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>219</v>
       </c>
@@ -3824,7 +3862,7 @@
       <c r="M91" s="14"/>
       <c r="S91" s="14"/>
     </row>
-    <row r="92" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>77</v>
       </c>
@@ -3847,7 +3885,7 @@
       <c r="M92" s="14"/>
       <c r="S92" s="14"/>
     </row>
-    <row r="93" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>79</v>
       </c>
@@ -3867,7 +3905,7 @@
       <c r="M93" s="14"/>
       <c r="S93" s="14"/>
     </row>
-    <row r="94" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>81</v>
       </c>
@@ -3890,7 +3928,7 @@
       <c r="M94" s="14"/>
       <c r="S94" s="14"/>
     </row>
-    <row r="95" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>84</v>
       </c>
@@ -3913,7 +3951,7 @@
       <c r="M95" s="14"/>
       <c r="S95" s="14"/>
     </row>
-    <row r="96" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>197</v>
       </c>
@@ -4008,6 +4046,9 @@
         <v>303</v>
       </c>
       <c r="S98" s="14"/>
+      <c r="T98" s="1" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="99" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
@@ -4114,6 +4155,7 @@
         <v>4</v>
       </c>
       <c r="S102" s="14"/>
+      <c r="T102" s="18"/>
     </row>
     <row r="103" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
@@ -4174,6 +4216,9 @@
         <v>16</v>
       </c>
       <c r="S104" s="14"/>
+      <c r="T104" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="105" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
@@ -4335,7 +4380,6 @@
       <c r="G111" s="14"/>
       <c r="M111" s="14"/>
       <c r="S111" s="14"/>
-      <c r="T111"/>
     </row>
     <row r="112" spans="1:20" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">

</xml_diff>

<commit_message>
Armatiek: niet standaard xmlschema genereren.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Armatiek/props/Armatiek.xlsx
+++ b/src/main/resources/input/Armatiek/props/Armatiek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Armatiek\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5944F6FC-89E0-43DD-891E-E82D741114D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657CAD3-B0DC-49D2-A0C6-6DCD07173A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="373">
   <si>
     <t>Name</t>
   </si>
@@ -1620,10 +1620,10 @@
   <dimension ref="A1:T133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="U44" sqref="U44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2423,7 +2423,7 @@
       <c r="M32" s="14"/>
       <c r="S32" s="14"/>
     </row>
-    <row r="33" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>265</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="M33" s="14"/>
       <c r="S33" s="14"/>
     </row>
-    <row r="34" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>325</v>
       </c>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="S34" s="14"/>
     </row>
-    <row r="35" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="M35" s="14"/>
       <c r="S35" s="14"/>
     </row>
-    <row r="36" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>170</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="M36" s="14"/>
       <c r="S36" s="14"/>
     </row>
-    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>173</v>
       </c>
@@ -2541,7 +2541,7 @@
       <c r="M37" s="14"/>
       <c r="S37" s="14"/>
     </row>
-    <row r="38" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>270</v>
       </c>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="S38" s="14"/>
     </row>
-    <row r="39" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2590,7 +2590,7 @@
       <c r="M39" s="14"/>
       <c r="S39" s="14"/>
     </row>
-    <row r="40" spans="1:19" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="18" t="s">
         <v>272</v>
       </c>
@@ -2625,7 +2625,7 @@
       <c r="M40" s="14"/>
       <c r="S40" s="14"/>
     </row>
-    <row r="41" spans="1:19" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="18" t="s">
         <v>342</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="M41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="M42" s="14"/>
       <c r="S42" s="14"/>
     </row>
-    <row r="43" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="M43" s="14"/>
       <c r="S43" s="14"/>
     </row>
-    <row r="44" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="1" t="s">
@@ -2737,8 +2737,11 @@
         <v>16</v>
       </c>
       <c r="S44" s="14"/>
-    </row>
-    <row r="45" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T44" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>264</v>
       </c>
@@ -2761,7 +2764,7 @@
       <c r="M45" s="14"/>
       <c r="S45" s="14"/>
     </row>
-    <row r="46" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>176</v>
       </c>
@@ -2784,7 +2787,7 @@
       <c r="M46" s="14"/>
       <c r="S46" s="14"/>
     </row>
-    <row r="47" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2807,7 +2810,7 @@
       <c r="M47" s="14"/>
       <c r="S47" s="14"/>
     </row>
-    <row r="48" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
OpenAPI als metamodel voor bootstrap van EA Toolbox generatie
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Armatiek/props/Armatiek.xlsx
+++ b/src/main/resources/input/Armatiek/props/Armatiek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Armatiek\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657CAD3-B0DC-49D2-A0C6-6DCD07173A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BB3131-71E5-43C1-B549-EB649466DE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="372">
   <si>
     <t>Name</t>
   </si>
@@ -1142,9 +1142,6 @@
   </si>
   <si>
     <t>BASE</t>
-  </si>
-  <si>
-    <t>API</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1617,10 @@
   <dimension ref="A1:T133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U44" sqref="U44"/>
+      <selection pane="bottomRight" activeCell="T99" sqref="T99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2053,7 +2050,7 @@
       </c>
       <c r="S16" s="14"/>
     </row>
-    <row r="17" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2076,7 +2073,7 @@
       <c r="M17" s="14"/>
       <c r="S17" s="14"/>
     </row>
-    <row r="18" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>223</v>
       </c>
@@ -2099,7 +2096,7 @@
       <c r="M18" s="14"/>
       <c r="S18" s="14"/>
     </row>
-    <row r="19" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>225</v>
       </c>
@@ -2118,7 +2115,7 @@
       <c r="M19" s="14"/>
       <c r="S19" s="14"/>
     </row>
-    <row r="20" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>166</v>
       </c>
@@ -2138,7 +2135,7 @@
       <c r="M20" s="14"/>
       <c r="S20" s="14"/>
     </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>138</v>
       </c>
@@ -2161,7 +2158,7 @@
       <c r="M21" s="14"/>
       <c r="S21" s="14"/>
     </row>
-    <row r="22" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>141</v>
       </c>
@@ -2184,7 +2181,7 @@
       <c r="M22" s="14"/>
       <c r="S22" s="14"/>
     </row>
-    <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>144</v>
       </c>
@@ -2213,7 +2210,7 @@
       </c>
       <c r="S23" s="14"/>
     </row>
-    <row r="24" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2236,7 +2233,7 @@
       <c r="M24" s="14"/>
       <c r="S24" s="14"/>
     </row>
-    <row r="25" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>168</v>
       </c>
@@ -2259,7 +2256,7 @@
       <c r="M25" s="14"/>
       <c r="S25" s="14"/>
     </row>
-    <row r="26" spans="1:19" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -2282,7 +2279,7 @@
       <c r="M26" s="14"/>
       <c r="S26" s="14"/>
     </row>
-    <row r="27" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -2305,7 +2302,7 @@
       <c r="M27" s="14"/>
       <c r="S27" s="14"/>
     </row>
-    <row r="28" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>322</v>
       </c>
@@ -2328,7 +2325,7 @@
       <c r="M28" s="14"/>
       <c r="S28" s="14"/>
     </row>
-    <row r="29" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>291</v>
       </c>
@@ -2351,7 +2348,7 @@
       <c r="M29" s="14"/>
       <c r="S29" s="14"/>
     </row>
-    <row r="30" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -2373,8 +2370,11 @@
       <c r="G30" s="14"/>
       <c r="M30" s="14"/>
       <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>146</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="M31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>260</v>
       </c>
@@ -2422,6 +2422,9 @@
       </c>
       <c r="M32" s="14"/>
       <c r="S32" s="14"/>
+      <c r="T32" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
@@ -2474,6 +2477,9 @@
         <v>16</v>
       </c>
       <c r="S34" s="14"/>
+      <c r="T34" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
@@ -2497,6 +2503,9 @@
       <c r="G35" s="14"/>
       <c r="M35" s="14"/>
       <c r="S35" s="14"/>
+      <c r="T35" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="36" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
@@ -2589,6 +2598,9 @@
       <c r="G39" s="14"/>
       <c r="M39" s="14"/>
       <c r="S39" s="14"/>
+      <c r="T39" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="18" t="s">
@@ -2624,6 +2636,9 @@
       </c>
       <c r="M40" s="14"/>
       <c r="S40" s="14"/>
+      <c r="T40" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="18" t="s">
@@ -3616,7 +3631,7 @@
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
       <c r="S82" s="14"/>
-      <c r="T82" s="1" t="s">
+      <c r="T82" s="4" t="s">
         <v>370</v>
       </c>
     </row>
@@ -4050,7 +4065,7 @@
       </c>
       <c r="S98" s="14"/>
       <c r="T98" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="99" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4636,6 +4651,9 @@
         <v>16</v>
       </c>
       <c r="S122" s="14"/>
+      <c r="T122" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="123" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">

</xml_diff>

<commit_message>
Armatiek: metamodel nature voor OpenAPI ingesteld
Dit is OPENAPI.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Armatiek/props/Armatiek.xlsx
+++ b/src/main/resources/input/Armatiek/props/Armatiek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Armatiek\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BB3131-71E5-43C1-B549-EB649466DE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DBAB42-8F08-4E51-9264-2AD6C685C606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="375">
   <si>
     <t>Name</t>
   </si>
@@ -1142,6 +1142,15 @@
   </si>
   <si>
     <t>BASE</t>
+  </si>
+  <si>
+    <t>metamodelnature</t>
+  </si>
+  <si>
+    <t>MIM;GROUPING</t>
+  </si>
+  <si>
+    <t>OPENAPI</t>
   </si>
 </sst>
 </file>
@@ -1614,13 +1623,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T133"/>
+  <dimension ref="A1:T134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T99" sqref="T99"/>
+      <selection pane="bottomRight" activeCell="T86" sqref="T86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3711,58 +3720,49 @@
         <v>370</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D85" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="1" t="b">
-        <v>1</v>
+        <v>372</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="G85" s="14"/>
       <c r="M85" s="14"/>
       <c r="S85" s="14"/>
-    </row>
-    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T85" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>329</v>
+        <v>196</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="D86" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="G86" s="14"/>
       <c r="M86" s="14"/>
       <c r="S86" s="14"/>
     </row>
-    <row r="87" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D87" s="1" t="b">
         <v>0</v>
@@ -3771,21 +3771,21 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>346</v>
+        <v>228</v>
       </c>
       <c r="G87" s="14"/>
       <c r="M87" s="14"/>
       <c r="S87" s="14"/>
     </row>
-    <row r="88" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D88" s="1" t="b">
         <v>0</v>
@@ -3794,321 +3794,321 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="G88" s="14"/>
       <c r="M88" s="14"/>
       <c r="S88" s="14"/>
     </row>
-    <row r="89" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D89" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>16</v>
+    <row r="89" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D89" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="G89" s="14"/>
       <c r="M89" s="14"/>
       <c r="S89" s="14"/>
     </row>
-    <row r="90" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="S90" s="14"/>
+    </row>
+    <row r="91" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D90" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G90" s="14"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
-      <c r="M90" s="14"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
-      <c r="S90" s="14"/>
-      <c r="T90" s="1"/>
-    </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="D91" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G91" s="14"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
       <c r="M91" s="14"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
       <c r="S91" s="14"/>
+      <c r="T91" s="1"/>
     </row>
     <row r="92" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="D92" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G92" s="14"/>
       <c r="M92" s="14"/>
       <c r="S92" s="14"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D93" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E93" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G93" s="14"/>
       <c r="M93" s="14"/>
       <c r="S93" s="14"/>
     </row>
-    <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D94" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>149</v>
+        <v>1</v>
       </c>
       <c r="G94" s="14"/>
       <c r="M94" s="14"/>
       <c r="S94" s="14"/>
     </row>
-    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D95" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>360</v>
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="G95" s="14"/>
       <c r="M95" s="14"/>
       <c r="S95" s="14"/>
     </row>
-    <row r="96" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D96" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>19</v>
+    <row r="96" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D96" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>360</v>
       </c>
       <c r="G96" s="14"/>
       <c r="M96" s="14"/>
       <c r="S96" s="14"/>
     </row>
-    <row r="97" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A97" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D97" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>213</v>
+    <row r="97" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G97" s="14"/>
       <c r="M97" s="14"/>
       <c r="S97" s="14"/>
     </row>
-    <row r="98" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D98" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="1" t="b">
-        <v>0</v>
+    <row r="98" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A98" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D98" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="G98" s="14"/>
-      <c r="H98" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="K98" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="L98" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="M98" s="14"/>
-      <c r="N98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="O98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="P98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R98" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="S98" s="14"/>
-      <c r="T98" s="1" t="s">
-        <v>369</v>
-      </c>
     </row>
     <row r="99" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D99" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" s="14"/>
+      <c r="H99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M99" s="14"/>
+      <c r="N99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="P99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S99" s="14"/>
+      <c r="T99" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D99" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="1" t="s">
+      <c r="D100" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G99" s="14"/>
-      <c r="M99" s="14"/>
-      <c r="S99" s="14"/>
-    </row>
-    <row r="100" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D100" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="G100" s="14"/>
       <c r="M100" s="14"/>
@@ -4116,140 +4116,119 @@
     </row>
     <row r="101" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D101" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E101" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="G101" s="14"/>
       <c r="M101" s="14"/>
       <c r="S101" s="14"/>
     </row>
     <row r="102" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="18" t="s">
+      <c r="A102" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D102" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="14"/>
+      <c r="M102" s="14"/>
+      <c r="S102" s="14"/>
+    </row>
+    <row r="103" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="B102" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="18" t="s">
+      <c r="B103" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="D102" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G102" s="14"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="18" t="s">
+      <c r="D103" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="14"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M102" s="19"/>
-      <c r="N102" s="18"/>
-      <c r="O102" s="18"/>
-      <c r="P102" s="18"/>
-      <c r="Q102" s="18"/>
-      <c r="R102" s="18" t="s">
+      <c r="M103" s="19"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+      <c r="R103" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S102" s="14"/>
-      <c r="T102" s="18"/>
-    </row>
-    <row r="103" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A103" s="1" t="s">
+      <c r="S103" s="14"/>
+      <c r="T103" s="18"/>
+    </row>
+    <row r="104" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A104" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D103" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="1" t="s">
+      <c r="D104" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G103" s="14"/>
-      <c r="M103" s="14"/>
-      <c r="S103" s="14"/>
-    </row>
-    <row r="104" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G104" s="14"/>
-      <c r="H104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L104" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M104" s="14"/>
-      <c r="N104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R104" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S104" s="14"/>
-      <c r="T104" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="105" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
       <c r="D105" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="1" t="b">
         <v>1</v>
@@ -4258,50 +4237,71 @@
         <v>4</v>
       </c>
       <c r="G105" s="14"/>
+      <c r="H105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M105" s="14"/>
+      <c r="N105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S105" s="14"/>
+      <c r="T105" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="106" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="D106" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>269</v>
+        <v>4</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
       <c r="S106" s="14"/>
     </row>
-    <row r="107" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>204</v>
+        <v>100</v>
       </c>
       <c r="D107" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="G107" s="14"/>
       <c r="M107" s="14"/>
@@ -4309,13 +4309,13 @@
     </row>
     <row r="108" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>248</v>
+        <v>202</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>250</v>
+        <v>204</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>0</v>
@@ -4323,31 +4323,31 @@
       <c r="E108" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="4" t="s">
-        <v>251</v>
+      <c r="F108" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="G108" s="14"/>
       <c r="M108" s="14"/>
       <c r="S108" s="14"/>
     </row>
-    <row r="109" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B109" t="s">
-        <v>10</v>
-      </c>
-      <c r="C109" t="s">
-        <v>276</v>
+        <v>248</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="D109" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>25</v>
+      <c r="F109" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="G109" s="14"/>
       <c r="M109" s="14"/>
@@ -4355,82 +4355,82 @@
     </row>
     <row r="110" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>5</v>
+        <v>222</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>348</v>
+        <v>276</v>
       </c>
       <c r="D110" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G110" s="14"/>
       <c r="M110" s="14"/>
       <c r="S110" s="14"/>
     </row>
-    <row r="111" spans="1:20" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>274</v>
-      </c>
-      <c r="B111" t="s">
-        <v>10</v>
+    <row r="111" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>275</v>
-      </c>
-      <c r="D111" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
-        <v>360</v>
+        <v>348</v>
+      </c>
+      <c r="D111" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="14"/>
       <c r="M111" s="14"/>
       <c r="S111" s="14"/>
     </row>
-    <row r="112" spans="1:20" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D112" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E112" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>16</v>
+    <row r="112" spans="1:20" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>274</v>
+      </c>
+      <c r="B112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" t="s">
+        <v>275</v>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>360</v>
       </c>
       <c r="G112" s="14"/>
       <c r="M112" s="14"/>
       <c r="S112" s="14"/>
     </row>
-    <row r="113" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:20" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D113" s="1" t="b">
         <v>0</v>
@@ -4438,22 +4438,22 @@
       <c r="E113" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F113" s="4" t="s">
-        <v>214</v>
+      <c r="F113" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G113" s="14"/>
       <c r="M113" s="14"/>
       <c r="S113" s="14"/>
     </row>
-    <row r="114" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>344</v>
+        <v>103</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>345</v>
+        <v>104</v>
       </c>
       <c r="D114" s="1" t="b">
         <v>0</v>
@@ -4462,21 +4462,21 @@
         <v>1</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>363</v>
+        <v>214</v>
       </c>
       <c r="G114" s="14"/>
       <c r="M114" s="14"/>
       <c r="S114" s="14"/>
     </row>
-    <row r="115" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>105</v>
+        <v>344</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>106</v>
+        <v>345</v>
       </c>
       <c r="D115" s="1" t="b">
         <v>0</v>
@@ -4484,28 +4484,31 @@
       <c r="E115" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>16</v>
+      <c r="F115" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="G115" s="14"/>
       <c r="M115" s="14"/>
       <c r="S115" s="14"/>
     </row>
-    <row r="116" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="D116" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E116" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G116" s="14"/>
       <c r="M116" s="14"/>
@@ -4513,65 +4516,62 @@
     </row>
     <row r="117" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="D117" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="G117" s="14"/>
       <c r="M117" s="14"/>
       <c r="S117" s="14"/>
     </row>
-    <row r="118" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D118" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G118" s="14"/>
       <c r="M118" s="14"/>
       <c r="S118" s="14"/>
     </row>
-    <row r="119" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D119" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>220</v>
+    <row r="119" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D119" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G119" s="14"/>
       <c r="M119" s="14"/>
@@ -4579,13 +4579,13 @@
     </row>
     <row r="120" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D120" s="5" t="b">
         <v>1</v>
@@ -4602,71 +4602,62 @@
     </row>
     <row r="121" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A121" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D121" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E121" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>16</v>
+        <v>220</v>
       </c>
       <c r="G121" s="14"/>
       <c r="M121" s="14"/>
       <c r="S121" s="14"/>
     </row>
-    <row r="122" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D122" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E122" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>4</v>
+    <row r="122" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D122" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G122" s="14"/>
-      <c r="H122" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M122" s="14"/>
-      <c r="N122" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S122" s="14"/>
-      <c r="T122" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="123" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D123" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123" s="1" t="b">
         <v>1</v>
@@ -4675,21 +4666,30 @@
         <v>4</v>
       </c>
       <c r="G123" s="14"/>
+      <c r="H123" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M123" s="14"/>
+      <c r="N123" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S123" s="14"/>
+      <c r="T123" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="124" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D124" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" s="1" t="b">
         <v>1</v>
@@ -4698,24 +4698,18 @@
         <v>4</v>
       </c>
       <c r="G124" s="14"/>
-      <c r="H124" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M124" s="14"/>
-      <c r="N124" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S124" s="14"/>
     </row>
-    <row r="125" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D125" s="1" t="b">
         <v>0</v>
@@ -4727,104 +4721,104 @@
         <v>4</v>
       </c>
       <c r="G125" s="14"/>
+      <c r="H125" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M125" s="14"/>
+      <c r="N125" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S125" s="14"/>
     </row>
-    <row r="126" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
+    <row r="126" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A126" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D126" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G126" s="14"/>
+      <c r="M126" s="14"/>
+      <c r="S126" s="14"/>
+    </row>
+    <row r="127" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
         <v>277</v>
       </c>
-      <c r="B126" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
         <v>278</v>
       </c>
-      <c r="D126" t="b">
-        <v>0</v>
-      </c>
-      <c r="E126" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" t="s">
+      <c r="D127" t="b">
+        <v>0</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127" t="s">
         <v>4</v>
       </c>
-      <c r="G126" s="14"/>
-      <c r="H126"/>
-      <c r="I126"/>
-      <c r="J126"/>
-      <c r="K126"/>
-      <c r="L126"/>
-      <c r="M126" s="17"/>
-      <c r="N126"/>
-      <c r="O126"/>
-      <c r="P126"/>
-      <c r="Q126"/>
-      <c r="R126"/>
-      <c r="S126" s="17"/>
-      <c r="T126"/>
-    </row>
-    <row r="127" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A127" s="5" t="s">
+      <c r="G127" s="14"/>
+      <c r="H127"/>
+      <c r="I127"/>
+      <c r="J127"/>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127" s="17"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127" s="17"/>
+      <c r="T127"/>
+    </row>
+    <row r="128" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A128" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B128" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C128" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D127" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E127" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G127" s="14"/>
-      <c r="M127" s="14"/>
-      <c r="S127" s="14"/>
-    </row>
-    <row r="128" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A128" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D128" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E128" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>4</v>
+      <c r="D128" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E128" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G128" s="14"/>
-      <c r="H128" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M128" s="14"/>
-      <c r="N128" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S128" s="14"/>
     </row>
     <row r="129" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>240</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D129" s="1" t="b">
         <v>1</v>
@@ -4847,92 +4841,121 @@
     </row>
     <row r="130" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>312</v>
+        <v>240</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="D130" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F130" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G130" s="14"/>
+      <c r="H130" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M130" s="14"/>
+      <c r="N130" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S130" s="14"/>
     </row>
     <row r="131" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
-        <v>131</v>
+        <v>312</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>132</v>
+        <v>313</v>
       </c>
       <c r="D131" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>360</v>
+        <v>1</v>
       </c>
       <c r="G131" s="14"/>
       <c r="M131" s="14"/>
       <c r="S131" s="14"/>
     </row>
-    <row r="132" spans="1:19" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
-        <v>257</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>258</v>
+        <v>132</v>
       </c>
       <c r="D132" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E132" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>259</v>
+        <v>360</v>
       </c>
       <c r="G132" s="14"/>
       <c r="M132" s="14"/>
       <c r="S132" s="14"/>
     </row>
-    <row r="133" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:19" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
-        <v>133</v>
+        <v>257</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>135</v>
+        <v>258</v>
       </c>
       <c r="D133" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E133" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="G133" s="14"/>
       <c r="M133" s="14"/>
       <c r="S133" s="14"/>
+    </row>
+    <row r="134" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D134" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E134" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G134" s="14"/>
+      <c r="M134" s="14"/>
+      <c r="S134" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>